<commit_message>
fixing branch step 2
</commit_message>
<xml_diff>
--- a/LR3/table_1_24.xlsx
+++ b/LR3/table_1_24.xlsx
@@ -1,24 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Студент\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IT\IT_LR\LR3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{67F156A3-8D61-4440-8ECC-65CE8DDB2A78}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8A56520E-246F-4E5C-AA23-D0AA97EC50CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{A4B6AF1B-B7A5-4949-8108-C54C638F128C}"/>
+    <workbookView xWindow="5835" yWindow="1755" windowWidth="21600" windowHeight="11385" xr2:uid="{A4B6AF1B-B7A5-4949-8108-C54C638F128C}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -228,7 +237,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -247,11 +256,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -259,26 +277,70 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="12">
     <dxf>
+      <font>
+        <b val="0"/>
+        <family val="1"/>
+      </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -299,37 +361,6 @@
         <scheme val="none"/>
       </font>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -346,17 +377,17 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0CDF27F8-8CCE-4966-84E4-CDF6947AAF4B}" name="Таблица2" displayName="Таблица2" ref="A2:K38" headerRowCount="0">
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{20ECBBB0-AEA3-4F9A-9191-072D87B0A1A3}" name="Столбец1" totalsRowLabel="Итог" headerRowDxfId="1" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{6570DA52-EFE7-4B93-BB6D-902823C08AEC}" name="Столбец2" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{20ECBBB0-AEA3-4F9A-9191-072D87B0A1A3}" name="Столбец1" totalsRowLabel="Итог" headerRowDxfId="11" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{6570DA52-EFE7-4B93-BB6D-902823C08AEC}" name="Столбец2" dataDxfId="1"/>
     <tableColumn id="3" xr3:uid="{256C28A8-C919-4CD9-BB9B-30430F003794}" name="Столбец3" dataDxfId="10"/>
     <tableColumn id="4" xr3:uid="{18A24A34-BC4F-4F32-AB98-0FA43F2CB4D4}" name="Столбец4" dataDxfId="9"/>
     <tableColumn id="5" xr3:uid="{6D45E14C-3992-4EAD-84D9-B7899E73D007}" name="Столбец5" dataDxfId="8"/>
     <tableColumn id="6" xr3:uid="{3297BC61-8C13-4FC1-82F8-D6DB2E269A2E}" name="Столбец6" dataDxfId="7"/>
     <tableColumn id="7" xr3:uid="{28F34830-B2A5-444A-BE69-6F69BE98D5A7}" name="Столбец7" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{65D0D6F4-98DD-468C-BF6D-B62872F990EB}" name="Столбец8" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{C0029E7A-8C97-4C68-83FE-CE0EC53A432E}" name="Столбец9" dataDxfId="5"/>
-    <tableColumn id="10" xr3:uid="{3537A7DB-DF4D-41DA-AE1D-A601B26AED92}" name="Столбец10" dataDxfId="4"/>
-    <tableColumn id="11" xr3:uid="{42865CC0-8744-485D-9AAE-59732AEB4BAD}" name="Столбец11" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{65D0D6F4-98DD-468C-BF6D-B62872F990EB}" name="Столбец8" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{C0029E7A-8C97-4C68-83FE-CE0EC53A432E}" name="Столбец9" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{3537A7DB-DF4D-41DA-AE1D-A601B26AED92}" name="Столбец10" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{42865CC0-8744-485D-9AAE-59732AEB4BAD}" name="Столбец11" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="1" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
 </table>
@@ -661,8 +692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00F402F3-B27D-431F-B447-93F9F2CC7A7E}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H42" sqref="H42"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -680,60 +711,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="2">
+      <c r="A1" s="4">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="2" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+      <c r="A3" s="9">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="4">
         <v>70</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="4">
         <f>1.1*4</f>
         <v>4.4000000000000004</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="4">
         <f>Таблица2[[#This Row],[Столбец3]]*Таблица2[[#This Row],[Столбец4]]</f>
         <v>308</v>
       </c>
@@ -743,37 +774,37 @@
       <c r="G3" s="7">
         <v>44805</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="4">
         <v>0</v>
       </c>
-      <c r="I3" s="1">
-        <v>10</v>
-      </c>
-      <c r="J3" s="1">
+      <c r="I3" s="4">
+        <v>10</v>
+      </c>
+      <c r="J3" s="4">
         <v>0</v>
       </c>
-      <c r="K3" s="1">
+      <c r="K3" s="4">
         <f>Таблица2[[#This Row],[Столбец10]]+Таблица2[[#This Row],[Столбец5]]</f>
         <v>308</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+      <c r="A4" s="9">
         <f>A3+1</f>
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="4">
         <f>C3-0.5</f>
         <v>69.5</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="4">
         <f>1.1*4</f>
         <v>4.4000000000000004</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="4">
         <f>Таблица2[[#This Row],[Столбец3]]*Таблица2[[#This Row],[Столбец4]]</f>
         <v>305.8</v>
       </c>
@@ -784,37 +815,37 @@
         <f>G3+1</f>
         <v>44806</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H4" s="4">
         <v>0</v>
       </c>
-      <c r="I4" s="1">
-        <v>10</v>
-      </c>
-      <c r="J4" s="1">
+      <c r="I4" s="4">
+        <v>10</v>
+      </c>
+      <c r="J4" s="4">
         <v>0</v>
       </c>
-      <c r="K4" s="1">
+      <c r="K4" s="4">
         <f>Таблица2[[#This Row],[Столбец10]]+Таблица2[[#This Row],[Столбец5]]</f>
         <v>305.8</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+      <c r="A5" s="9">
         <f t="shared" ref="A5:A38" si="0">A4+1</f>
         <v>3</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="4">
         <f t="shared" ref="C5:C38" si="1">C4-0.5</f>
         <v>69</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="4">
         <f t="shared" ref="D5:D38" si="2">1.1*4</f>
         <v>4.4000000000000004</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="4">
         <f>Таблица2[[#This Row],[Столбец3]]*Таблица2[[#This Row],[Столбец4]]</f>
         <v>303.60000000000002</v>
       </c>
@@ -825,37 +856,37 @@
         <f t="shared" ref="G5:G31" si="3">G4+1</f>
         <v>44807</v>
       </c>
-      <c r="H5" s="1">
+      <c r="H5" s="4">
         <v>0</v>
       </c>
-      <c r="I5" s="1">
-        <v>10</v>
-      </c>
-      <c r="J5" s="1">
+      <c r="I5" s="4">
+        <v>10</v>
+      </c>
+      <c r="J5" s="4">
         <v>0</v>
       </c>
-      <c r="K5" s="1">
+      <c r="K5" s="4">
         <f>Таблица2[[#This Row],[Столбец10]]+Таблица2[[#This Row],[Столбец5]]</f>
         <v>303.60000000000002</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+      <c r="A6" s="9">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="4">
         <f t="shared" si="1"/>
         <v>68.5</v>
       </c>
-      <c r="D6" s="1">
-        <f t="shared" si="2"/>
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="E6" s="1">
+      <c r="D6" s="4">
+        <f t="shared" si="2"/>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E6" s="4">
         <f>Таблица2[[#This Row],[Столбец3]]*Таблица2[[#This Row],[Столбец4]]</f>
         <v>301.40000000000003</v>
       </c>
@@ -866,37 +897,37 @@
         <f t="shared" si="3"/>
         <v>44808</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6" s="4">
         <v>0</v>
       </c>
-      <c r="I6" s="1">
-        <v>10</v>
-      </c>
-      <c r="J6" s="1">
+      <c r="I6" s="4">
+        <v>10</v>
+      </c>
+      <c r="J6" s="4">
         <v>0</v>
       </c>
-      <c r="K6" s="1">
+      <c r="K6" s="4">
         <f>Таблица2[[#This Row],[Столбец10]]+Таблица2[[#This Row],[Столбец5]]</f>
         <v>301.40000000000003</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+      <c r="A7" s="9">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="4">
         <f t="shared" si="1"/>
         <v>68</v>
       </c>
-      <c r="D7" s="1">
-        <f t="shared" si="2"/>
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="E7" s="1">
+      <c r="D7" s="4">
+        <f t="shared" si="2"/>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E7" s="4">
         <f>Таблица2[[#This Row],[Столбец3]]*Таблица2[[#This Row],[Столбец4]]</f>
         <v>299.20000000000005</v>
       </c>
@@ -907,37 +938,37 @@
         <f t="shared" si="3"/>
         <v>44809</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H7" s="4">
         <v>0</v>
       </c>
-      <c r="I7" s="1">
-        <v>10</v>
-      </c>
-      <c r="J7" s="1">
+      <c r="I7" s="4">
+        <v>10</v>
+      </c>
+      <c r="J7" s="4">
         <v>0</v>
       </c>
-      <c r="K7" s="1">
+      <c r="K7" s="4">
         <f>Таблица2[[#This Row],[Столбец10]]+Таблица2[[#This Row],[Столбец5]]</f>
         <v>299.20000000000005</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+      <c r="A8" s="9">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="4">
         <f t="shared" si="1"/>
         <v>67.5</v>
       </c>
-      <c r="D8" s="1">
-        <f t="shared" si="2"/>
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="E8" s="1">
+      <c r="D8" s="4">
+        <f t="shared" si="2"/>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E8" s="4">
         <f>Таблица2[[#This Row],[Столбец3]]*Таблица2[[#This Row],[Столбец4]]</f>
         <v>297</v>
       </c>
@@ -948,37 +979,37 @@
         <f t="shared" si="3"/>
         <v>44810</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H8" s="4">
         <v>0</v>
       </c>
-      <c r="I8" s="1">
-        <v>10</v>
-      </c>
-      <c r="J8" s="1">
+      <c r="I8" s="4">
+        <v>10</v>
+      </c>
+      <c r="J8" s="4">
         <v>0</v>
       </c>
-      <c r="K8" s="1">
+      <c r="K8" s="4">
         <f>Таблица2[[#This Row],[Столбец10]]+Таблица2[[#This Row],[Столбец5]]</f>
         <v>297</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
+      <c r="A9" s="9">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="4">
         <f t="shared" si="1"/>
         <v>67</v>
       </c>
-      <c r="D9" s="1">
-        <f t="shared" si="2"/>
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="E9" s="1">
+      <c r="D9" s="4">
+        <f t="shared" si="2"/>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E9" s="4">
         <f>Таблица2[[#This Row],[Столбец3]]*Таблица2[[#This Row],[Столбец4]]</f>
         <v>294.8</v>
       </c>
@@ -989,37 +1020,37 @@
         <f t="shared" si="3"/>
         <v>44811</v>
       </c>
-      <c r="H9" s="1">
+      <c r="H9" s="4">
         <v>0</v>
       </c>
-      <c r="I9" s="1">
-        <v>10</v>
-      </c>
-      <c r="J9" s="1">
+      <c r="I9" s="4">
+        <v>10</v>
+      </c>
+      <c r="J9" s="4">
         <v>0</v>
       </c>
-      <c r="K9" s="1">
+      <c r="K9" s="4">
         <f>Таблица2[[#This Row],[Столбец10]]+Таблица2[[#This Row],[Столбец5]]</f>
         <v>294.8</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
+      <c r="A10" s="9">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="4">
         <f t="shared" si="1"/>
         <v>66.5</v>
       </c>
-      <c r="D10" s="1">
-        <f t="shared" si="2"/>
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="E10" s="1">
+      <c r="D10" s="4">
+        <f t="shared" si="2"/>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E10" s="4">
         <f>Таблица2[[#This Row],[Столбец3]]*Таблица2[[#This Row],[Столбец4]]</f>
         <v>292.60000000000002</v>
       </c>
@@ -1030,37 +1061,37 @@
         <f t="shared" si="3"/>
         <v>44812</v>
       </c>
-      <c r="H10" s="1">
+      <c r="H10" s="4">
         <v>0</v>
       </c>
-      <c r="I10" s="1">
-        <v>10</v>
-      </c>
-      <c r="J10" s="1">
+      <c r="I10" s="4">
+        <v>10</v>
+      </c>
+      <c r="J10" s="4">
         <v>0</v>
       </c>
-      <c r="K10" s="1">
+      <c r="K10" s="4">
         <f>Таблица2[[#This Row],[Столбец10]]+Таблица2[[#This Row],[Столбец5]]</f>
         <v>292.60000000000002</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
+      <c r="A11" s="9">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="1">
+      <c r="B11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="4">
         <f t="shared" si="1"/>
         <v>66</v>
       </c>
-      <c r="D11" s="1">
-        <f t="shared" si="2"/>
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="E11" s="1">
+      <c r="D11" s="4">
+        <f t="shared" si="2"/>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E11" s="4">
         <f>Таблица2[[#This Row],[Столбец3]]*Таблица2[[#This Row],[Столбец4]]</f>
         <v>290.40000000000003</v>
       </c>
@@ -1071,37 +1102,37 @@
         <f t="shared" si="3"/>
         <v>44813</v>
       </c>
-      <c r="H11" s="1">
+      <c r="H11" s="4">
         <v>0</v>
       </c>
-      <c r="I11" s="1">
-        <v>10</v>
-      </c>
-      <c r="J11" s="1">
+      <c r="I11" s="4">
+        <v>10</v>
+      </c>
+      <c r="J11" s="4">
         <v>0</v>
       </c>
-      <c r="K11" s="1">
+      <c r="K11" s="4">
         <f>Таблица2[[#This Row],[Столбец10]]+Таблица2[[#This Row],[Столбец5]]</f>
         <v>290.40000000000003</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="B12" s="1" t="s">
+      <c r="A12" s="9">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="4">
         <f t="shared" si="1"/>
         <v>65.5</v>
       </c>
-      <c r="D12" s="1">
-        <f t="shared" si="2"/>
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="E12" s="1">
+      <c r="D12" s="4">
+        <f t="shared" si="2"/>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E12" s="4">
         <f>Таблица2[[#This Row],[Столбец3]]*Таблица2[[#This Row],[Столбец4]]</f>
         <v>288.20000000000005</v>
       </c>
@@ -1112,38 +1143,38 @@
         <f t="shared" si="3"/>
         <v>44814</v>
       </c>
-      <c r="H12" s="1">
+      <c r="H12" s="4">
         <v>1</v>
       </c>
-      <c r="I12" s="1">
-        <v>10</v>
-      </c>
-      <c r="J12" s="1">
-        <f>Таблица2[[#This Row],[Столбец9]]*Таблица2[[#This Row],[Столбец8]]</f>
-        <v>10</v>
-      </c>
-      <c r="K12" s="1">
+      <c r="I12" s="4">
+        <v>10</v>
+      </c>
+      <c r="J12" s="4">
+        <f>Таблица2[[#This Row],[Столбец9]]*Таблица2[[#This Row],[Столбец8]]</f>
+        <v>10</v>
+      </c>
+      <c r="K12" s="4">
         <f>Таблица2[[#This Row],[Столбец10]]+Таблица2[[#This Row],[Столбец5]]</f>
         <v>298.20000000000005</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
+      <c r="A13" s="9">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="4">
         <f t="shared" si="1"/>
         <v>65</v>
       </c>
-      <c r="D13" s="1">
-        <f t="shared" si="2"/>
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="E13" s="1">
+      <c r="D13" s="4">
+        <f t="shared" si="2"/>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E13" s="4">
         <f>Таблица2[[#This Row],[Столбец3]]*Таблица2[[#This Row],[Столбец4]]</f>
         <v>286</v>
       </c>
@@ -1154,39 +1185,39 @@
         <f t="shared" si="3"/>
         <v>44815</v>
       </c>
-      <c r="H13" s="1">
+      <c r="H13" s="4">
         <f>H12+1</f>
         <v>2</v>
       </c>
-      <c r="I13" s="1">
-        <v>10</v>
-      </c>
-      <c r="J13" s="1">
+      <c r="I13" s="4">
+        <v>10</v>
+      </c>
+      <c r="J13" s="4">
         <f>Таблица2[[#This Row],[Столбец9]]*Таблица2[[#This Row],[Столбец8]]</f>
         <v>20</v>
       </c>
-      <c r="K13" s="1">
+      <c r="K13" s="4">
         <f>Таблица2[[#This Row],[Столбец10]]+Таблица2[[#This Row],[Столбец5]]</f>
         <v>306</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
+      <c r="A14" s="9">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="4">
         <f t="shared" si="1"/>
         <v>64.5</v>
       </c>
-      <c r="D14" s="1">
-        <f t="shared" si="2"/>
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="E14" s="1">
+      <c r="D14" s="4">
+        <f t="shared" si="2"/>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E14" s="4">
         <f>Таблица2[[#This Row],[Столбец3]]*Таблица2[[#This Row],[Столбец4]]</f>
         <v>283.8</v>
       </c>
@@ -1197,39 +1228,39 @@
         <f t="shared" si="3"/>
         <v>44816</v>
       </c>
-      <c r="H14" s="1">
+      <c r="H14" s="4">
         <f t="shared" ref="H14:H38" si="4">H13+1</f>
         <v>3</v>
       </c>
-      <c r="I14" s="1">
-        <v>10</v>
-      </c>
-      <c r="J14" s="1">
+      <c r="I14" s="4">
+        <v>10</v>
+      </c>
+      <c r="J14" s="4">
         <f>Таблица2[[#This Row],[Столбец9]]*Таблица2[[#This Row],[Столбец8]]</f>
         <v>30</v>
       </c>
-      <c r="K14" s="1">
+      <c r="K14" s="4">
         <f>Таблица2[[#This Row],[Столбец10]]+Таблица2[[#This Row],[Столбец5]]</f>
         <v>313.8</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
+      <c r="A15" s="9">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="4">
         <f t="shared" si="1"/>
         <v>64</v>
       </c>
-      <c r="D15" s="1">
-        <f t="shared" si="2"/>
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="E15" s="1">
+      <c r="D15" s="4">
+        <f t="shared" si="2"/>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E15" s="4">
         <f>Таблица2[[#This Row],[Столбец3]]*Таблица2[[#This Row],[Столбец4]]</f>
         <v>281.60000000000002</v>
       </c>
@@ -1240,39 +1271,39 @@
         <f t="shared" si="3"/>
         <v>44817</v>
       </c>
-      <c r="H15" s="1">
+      <c r="H15" s="4">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="I15" s="1">
-        <v>10</v>
-      </c>
-      <c r="J15" s="1">
+      <c r="I15" s="4">
+        <v>10</v>
+      </c>
+      <c r="J15" s="4">
         <f>Таблица2[[#This Row],[Столбец9]]*Таблица2[[#This Row],[Столбец8]]</f>
         <v>40</v>
       </c>
-      <c r="K15" s="1">
+      <c r="K15" s="4">
         <f>Таблица2[[#This Row],[Столбец10]]+Таблица2[[#This Row],[Столбец5]]</f>
         <v>321.60000000000002</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
+      <c r="A16" s="9">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="4">
         <f t="shared" si="1"/>
         <v>63.5</v>
       </c>
-      <c r="D16" s="1">
-        <f t="shared" si="2"/>
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="E16" s="1">
+      <c r="D16" s="4">
+        <f t="shared" si="2"/>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E16" s="4">
         <f>Таблица2[[#This Row],[Столбец3]]*Таблица2[[#This Row],[Столбец4]]</f>
         <v>279.40000000000003</v>
       </c>
@@ -1283,39 +1314,39 @@
         <f t="shared" si="3"/>
         <v>44818</v>
       </c>
-      <c r="H16" s="1">
+      <c r="H16" s="4">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="I16" s="1">
-        <v>10</v>
-      </c>
-      <c r="J16" s="1">
+      <c r="I16" s="4">
+        <v>10</v>
+      </c>
+      <c r="J16" s="4">
         <f>Таблица2[[#This Row],[Столбец9]]*Таблица2[[#This Row],[Столбец8]]</f>
         <v>50</v>
       </c>
-      <c r="K16" s="1">
+      <c r="K16" s="4">
         <f>Таблица2[[#This Row],[Столбец10]]+Таблица2[[#This Row],[Столбец5]]</f>
         <v>329.40000000000003</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
+      <c r="A17" s="9">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="4">
         <f t="shared" si="1"/>
         <v>63</v>
       </c>
-      <c r="D17" s="1">
-        <f t="shared" si="2"/>
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="E17" s="1">
+      <c r="D17" s="4">
+        <f t="shared" si="2"/>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E17" s="4">
         <f>Таблица2[[#This Row],[Столбец3]]*Таблица2[[#This Row],[Столбец4]]</f>
         <v>277.20000000000005</v>
       </c>
@@ -1326,39 +1357,39 @@
         <f t="shared" si="3"/>
         <v>44819</v>
       </c>
-      <c r="H17" s="1">
+      <c r="H17" s="4">
         <f t="shared" si="4"/>
         <v>6</v>
       </c>
-      <c r="I17" s="1">
-        <v>10</v>
-      </c>
-      <c r="J17" s="1">
+      <c r="I17" s="4">
+        <v>10</v>
+      </c>
+      <c r="J17" s="4">
         <f>Таблица2[[#This Row],[Столбец9]]*Таблица2[[#This Row],[Столбец8]]</f>
         <v>60</v>
       </c>
-      <c r="K17" s="1">
+      <c r="K17" s="4">
         <f>Таблица2[[#This Row],[Столбец10]]+Таблица2[[#This Row],[Столбец5]]</f>
         <v>337.20000000000005</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
+      <c r="A18" s="9">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="4">
         <f t="shared" si="1"/>
         <v>62.5</v>
       </c>
-      <c r="D18" s="1">
-        <f t="shared" si="2"/>
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="E18" s="1">
+      <c r="D18" s="4">
+        <f t="shared" si="2"/>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E18" s="4">
         <f>Таблица2[[#This Row],[Столбец3]]*Таблица2[[#This Row],[Столбец4]]</f>
         <v>275</v>
       </c>
@@ -1369,39 +1400,39 @@
         <f t="shared" si="3"/>
         <v>44820</v>
       </c>
-      <c r="H18" s="1">
+      <c r="H18" s="4">
         <f t="shared" si="4"/>
         <v>7</v>
       </c>
-      <c r="I18" s="1">
-        <v>10</v>
-      </c>
-      <c r="J18" s="1">
+      <c r="I18" s="4">
+        <v>10</v>
+      </c>
+      <c r="J18" s="4">
         <f>Таблица2[[#This Row],[Столбец9]]*Таблица2[[#This Row],[Столбец8]]</f>
         <v>70</v>
       </c>
-      <c r="K18" s="1">
+      <c r="K18" s="4">
         <f>Таблица2[[#This Row],[Столбец10]]+Таблица2[[#This Row],[Столбец5]]</f>
         <v>345</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
+      <c r="A19" s="9">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19" s="4">
         <f t="shared" si="1"/>
         <v>62</v>
       </c>
-      <c r="D19" s="1">
-        <f t="shared" si="2"/>
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="E19" s="1">
+      <c r="D19" s="4">
+        <f t="shared" si="2"/>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E19" s="4">
         <f>Таблица2[[#This Row],[Столбец3]]*Таблица2[[#This Row],[Столбец4]]</f>
         <v>272.8</v>
       </c>
@@ -1412,39 +1443,39 @@
         <f t="shared" si="3"/>
         <v>44821</v>
       </c>
-      <c r="H19" s="1">
+      <c r="H19" s="4">
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
-      <c r="I19" s="1">
-        <v>10</v>
-      </c>
-      <c r="J19" s="1">
+      <c r="I19" s="4">
+        <v>10</v>
+      </c>
+      <c r="J19" s="4">
         <f>Таблица2[[#This Row],[Столбец9]]*Таблица2[[#This Row],[Столбец8]]</f>
         <v>80</v>
       </c>
-      <c r="K19" s="1">
+      <c r="K19" s="4">
         <f>Таблица2[[#This Row],[Столбец10]]+Таблица2[[#This Row],[Столбец5]]</f>
         <v>352.8</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
+      <c r="A20" s="9">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20" s="4">
         <f t="shared" si="1"/>
         <v>61.5</v>
       </c>
-      <c r="D20" s="1">
-        <f t="shared" si="2"/>
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="E20" s="1">
+      <c r="D20" s="4">
+        <f t="shared" si="2"/>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E20" s="4">
         <f>Таблица2[[#This Row],[Столбец3]]*Таблица2[[#This Row],[Столбец4]]</f>
         <v>270.60000000000002</v>
       </c>
@@ -1455,39 +1486,39 @@
         <f t="shared" si="3"/>
         <v>44822</v>
       </c>
-      <c r="H20" s="1">
+      <c r="H20" s="4">
         <f t="shared" si="4"/>
         <v>9</v>
       </c>
-      <c r="I20" s="1">
-        <v>10</v>
-      </c>
-      <c r="J20" s="1">
+      <c r="I20" s="4">
+        <v>10</v>
+      </c>
+      <c r="J20" s="4">
         <f>Таблица2[[#This Row],[Столбец9]]*Таблица2[[#This Row],[Столбец8]]</f>
         <v>90</v>
       </c>
-      <c r="K20" s="1">
+      <c r="K20" s="4">
         <f>Таблица2[[#This Row],[Столбец10]]+Таблица2[[#This Row],[Столбец5]]</f>
         <v>360.6</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
+      <c r="A21" s="9">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21" s="4">
         <f t="shared" si="1"/>
         <v>61</v>
       </c>
-      <c r="D21" s="1">
-        <f t="shared" si="2"/>
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="E21" s="1">
+      <c r="D21" s="4">
+        <f t="shared" si="2"/>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E21" s="4">
         <f>Таблица2[[#This Row],[Столбец3]]*Таблица2[[#This Row],[Столбец4]]</f>
         <v>268.40000000000003</v>
       </c>
@@ -1498,39 +1529,39 @@
         <f t="shared" si="3"/>
         <v>44823</v>
       </c>
-      <c r="H21" s="1">
+      <c r="H21" s="4">
         <f t="shared" si="4"/>
         <v>10</v>
       </c>
-      <c r="I21" s="1">
-        <v>10</v>
-      </c>
-      <c r="J21" s="1">
+      <c r="I21" s="4">
+        <v>10</v>
+      </c>
+      <c r="J21" s="4">
         <f>Таблица2[[#This Row],[Столбец9]]*Таблица2[[#This Row],[Столбец8]]</f>
         <v>100</v>
       </c>
-      <c r="K21" s="1">
+      <c r="K21" s="4">
         <f>Таблица2[[#This Row],[Столбец10]]+Таблица2[[#This Row],[Столбец5]]</f>
         <v>368.40000000000003</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
+      <c r="A22" s="9">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C22" s="4">
         <f t="shared" si="1"/>
         <v>60.5</v>
       </c>
-      <c r="D22" s="1">
-        <f t="shared" si="2"/>
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="E22" s="1">
+      <c r="D22" s="4">
+        <f t="shared" si="2"/>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E22" s="4">
         <f>Таблица2[[#This Row],[Столбец3]]*Таблица2[[#This Row],[Столбец4]]</f>
         <v>266.20000000000005</v>
       </c>
@@ -1541,39 +1572,39 @@
         <f t="shared" si="3"/>
         <v>44824</v>
       </c>
-      <c r="H22" s="1">
+      <c r="H22" s="4">
         <f t="shared" si="4"/>
         <v>11</v>
       </c>
-      <c r="I22" s="1">
-        <v>10</v>
-      </c>
-      <c r="J22" s="1">
+      <c r="I22" s="4">
+        <v>10</v>
+      </c>
+      <c r="J22" s="4">
         <f>Таблица2[[#This Row],[Столбец9]]*Таблица2[[#This Row],[Столбец8]]</f>
         <v>110</v>
       </c>
-      <c r="K22" s="1">
+      <c r="K22" s="4">
         <f>Таблица2[[#This Row],[Столбец10]]+Таблица2[[#This Row],[Столбец5]]</f>
         <v>376.20000000000005</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
+      <c r="A23" s="9">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23" s="4">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="D23" s="1">
-        <f t="shared" si="2"/>
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="E23" s="1">
+      <c r="D23" s="4">
+        <f t="shared" si="2"/>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E23" s="4">
         <f>Таблица2[[#This Row],[Столбец3]]*Таблица2[[#This Row],[Столбец4]]</f>
         <v>264</v>
       </c>
@@ -1584,39 +1615,39 @@
         <f>G22+1</f>
         <v>44825</v>
       </c>
-      <c r="H23" s="1">
+      <c r="H23" s="4">
         <f t="shared" si="4"/>
         <v>12</v>
       </c>
-      <c r="I23" s="1">
-        <v>10</v>
-      </c>
-      <c r="J23" s="1">
+      <c r="I23" s="4">
+        <v>10</v>
+      </c>
+      <c r="J23" s="4">
         <f>Таблица2[[#This Row],[Столбец9]]*Таблица2[[#This Row],[Столбец8]]</f>
         <v>120</v>
       </c>
-      <c r="K23" s="1">
+      <c r="K23" s="4">
         <f>Таблица2[[#This Row],[Столбец10]]+Таблица2[[#This Row],[Столбец5]]</f>
         <v>384</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
+      <c r="A24" s="9">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="4">
         <f t="shared" si="1"/>
         <v>59.5</v>
       </c>
-      <c r="D24" s="1">
-        <f t="shared" si="2"/>
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="E24" s="1">
+      <c r="D24" s="4">
+        <f t="shared" si="2"/>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E24" s="4">
         <f>Таблица2[[#This Row],[Столбец3]]*Таблица2[[#This Row],[Столбец4]]</f>
         <v>261.8</v>
       </c>
@@ -1627,39 +1658,39 @@
         <f t="shared" si="3"/>
         <v>44826</v>
       </c>
-      <c r="H24" s="1">
+      <c r="H24" s="4">
         <f t="shared" si="4"/>
         <v>13</v>
       </c>
-      <c r="I24" s="1">
-        <v>10</v>
-      </c>
-      <c r="J24" s="1">
+      <c r="I24" s="4">
+        <v>10</v>
+      </c>
+      <c r="J24" s="4">
         <f>Таблица2[[#This Row],[Столбец9]]*Таблица2[[#This Row],[Столбец8]]</f>
         <v>130</v>
       </c>
-      <c r="K24" s="1">
+      <c r="K24" s="4">
         <f>Таблица2[[#This Row],[Столбец10]]+Таблица2[[#This Row],[Столбец5]]</f>
         <v>391.8</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
+      <c r="A25" s="9">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25" s="4">
         <f t="shared" si="1"/>
         <v>59</v>
       </c>
-      <c r="D25" s="1">
-        <f t="shared" si="2"/>
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="E25" s="1">
+      <c r="D25" s="4">
+        <f t="shared" si="2"/>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E25" s="4">
         <f>Таблица2[[#This Row],[Столбец3]]*Таблица2[[#This Row],[Столбец4]]</f>
         <v>259.60000000000002</v>
       </c>
@@ -1670,39 +1701,39 @@
         <f t="shared" si="3"/>
         <v>44827</v>
       </c>
-      <c r="H25" s="1">
+      <c r="H25" s="4">
         <f t="shared" si="4"/>
         <v>14</v>
       </c>
-      <c r="I25" s="1">
-        <v>10</v>
-      </c>
-      <c r="J25" s="1">
+      <c r="I25" s="4">
+        <v>10</v>
+      </c>
+      <c r="J25" s="4">
         <f>Таблица2[[#This Row],[Столбец9]]*Таблица2[[#This Row],[Столбец8]]</f>
         <v>140</v>
       </c>
-      <c r="K25" s="1">
+      <c r="K25" s="4">
         <f>Таблица2[[#This Row],[Столбец10]]+Таблица2[[#This Row],[Столбец5]]</f>
         <v>399.6</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
+      <c r="A26" s="9">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26" s="4">
         <f t="shared" si="1"/>
         <v>58.5</v>
       </c>
-      <c r="D26" s="1">
-        <f t="shared" si="2"/>
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="E26" s="1">
+      <c r="D26" s="4">
+        <f t="shared" si="2"/>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E26" s="4">
         <f>Таблица2[[#This Row],[Столбец3]]*Таблица2[[#This Row],[Столбец4]]</f>
         <v>257.40000000000003</v>
       </c>
@@ -1713,39 +1744,39 @@
         <f t="shared" si="3"/>
         <v>44828</v>
       </c>
-      <c r="H26" s="1">
+      <c r="H26" s="4">
         <f t="shared" si="4"/>
         <v>15</v>
       </c>
-      <c r="I26" s="1">
-        <v>10</v>
-      </c>
-      <c r="J26" s="1">
+      <c r="I26" s="4">
+        <v>10</v>
+      </c>
+      <c r="J26" s="4">
         <f>Таблица2[[#This Row],[Столбец9]]*Таблица2[[#This Row],[Столбец8]]</f>
         <v>150</v>
       </c>
-      <c r="K26" s="1">
+      <c r="K26" s="4">
         <f>Таблица2[[#This Row],[Столбец10]]+Таблица2[[#This Row],[Столбец5]]</f>
         <v>407.40000000000003</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
+      <c r="A27" s="9">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27" s="4">
         <f t="shared" si="1"/>
         <v>58</v>
       </c>
-      <c r="D27" s="1">
-        <f t="shared" si="2"/>
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="E27" s="1">
+      <c r="D27" s="4">
+        <f t="shared" si="2"/>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E27" s="4">
         <f>Таблица2[[#This Row],[Столбец3]]*Таблица2[[#This Row],[Столбец4]]</f>
         <v>255.20000000000002</v>
       </c>
@@ -1756,39 +1787,39 @@
         <f t="shared" si="3"/>
         <v>44829</v>
       </c>
-      <c r="H27" s="1">
+      <c r="H27" s="4">
         <f t="shared" si="4"/>
         <v>16</v>
       </c>
-      <c r="I27" s="1">
-        <v>10</v>
-      </c>
-      <c r="J27" s="1">
+      <c r="I27" s="4">
+        <v>10</v>
+      </c>
+      <c r="J27" s="4">
         <f>Таблица2[[#This Row],[Столбец9]]*Таблица2[[#This Row],[Столбец8]]</f>
         <v>160</v>
       </c>
-      <c r="K27" s="1">
+      <c r="K27" s="4">
         <f>Таблица2[[#This Row],[Столбец10]]+Таблица2[[#This Row],[Столбец5]]</f>
         <v>415.20000000000005</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
+      <c r="A28" s="9">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C28" s="4">
         <f t="shared" si="1"/>
         <v>57.5</v>
       </c>
-      <c r="D28" s="1">
-        <f t="shared" si="2"/>
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="E28" s="1">
+      <c r="D28" s="4">
+        <f t="shared" si="2"/>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E28" s="4">
         <f>Таблица2[[#This Row],[Столбец3]]*Таблица2[[#This Row],[Столбец4]]</f>
         <v>253.00000000000003</v>
       </c>
@@ -1799,39 +1830,39 @@
         <f t="shared" si="3"/>
         <v>44830</v>
       </c>
-      <c r="H28" s="1">
+      <c r="H28" s="4">
         <f t="shared" si="4"/>
         <v>17</v>
       </c>
-      <c r="I28" s="1">
-        <v>10</v>
-      </c>
-      <c r="J28" s="1">
+      <c r="I28" s="4">
+        <v>10</v>
+      </c>
+      <c r="J28" s="4">
         <f>Таблица2[[#This Row],[Столбец9]]*Таблица2[[#This Row],[Столбец8]]</f>
         <v>170</v>
       </c>
-      <c r="K28" s="1">
+      <c r="K28" s="4">
         <f>Таблица2[[#This Row],[Столбец10]]+Таблица2[[#This Row],[Столбец5]]</f>
         <v>423</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
+      <c r="A29" s="9">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C29" s="4">
         <f t="shared" si="1"/>
         <v>57</v>
       </c>
-      <c r="D29" s="1">
-        <f t="shared" si="2"/>
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="E29" s="1">
+      <c r="D29" s="4">
+        <f t="shared" si="2"/>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E29" s="4">
         <f>Таблица2[[#This Row],[Столбец3]]*Таблица2[[#This Row],[Столбец4]]</f>
         <v>250.8</v>
       </c>
@@ -1842,39 +1873,39 @@
         <f t="shared" si="3"/>
         <v>44831</v>
       </c>
-      <c r="H29" s="1">
+      <c r="H29" s="4">
         <f t="shared" si="4"/>
         <v>18</v>
       </c>
-      <c r="I29" s="1">
-        <v>10</v>
-      </c>
-      <c r="J29" s="1">
+      <c r="I29" s="4">
+        <v>10</v>
+      </c>
+      <c r="J29" s="4">
         <f>Таблица2[[#This Row],[Столбец9]]*Таблица2[[#This Row],[Столбец8]]</f>
         <v>180</v>
       </c>
-      <c r="K29" s="1">
+      <c r="K29" s="4">
         <f>Таблица2[[#This Row],[Столбец10]]+Таблица2[[#This Row],[Столбец5]]</f>
         <v>430.8</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
+      <c r="A30" s="9">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C30" s="4">
         <f t="shared" si="1"/>
         <v>56.5</v>
       </c>
-      <c r="D30" s="1">
-        <f t="shared" si="2"/>
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="E30" s="1">
+      <c r="D30" s="4">
+        <f t="shared" si="2"/>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E30" s="4">
         <f>Таблица2[[#This Row],[Столбец3]]*Таблица2[[#This Row],[Столбец4]]</f>
         <v>248.60000000000002</v>
       </c>
@@ -1885,39 +1916,39 @@
         <f>G29+1</f>
         <v>44832</v>
       </c>
-      <c r="H30" s="1">
+      <c r="H30" s="4">
         <f t="shared" si="4"/>
         <v>19</v>
       </c>
-      <c r="I30" s="1">
-        <v>10</v>
-      </c>
-      <c r="J30" s="1">
+      <c r="I30" s="4">
+        <v>10</v>
+      </c>
+      <c r="J30" s="4">
         <f>Таблица2[[#This Row],[Столбец9]]*Таблица2[[#This Row],[Столбец8]]</f>
         <v>190</v>
       </c>
-      <c r="K30" s="1">
+      <c r="K30" s="4">
         <f>Таблица2[[#This Row],[Столбец10]]+Таблица2[[#This Row],[Столбец5]]</f>
         <v>438.6</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
+      <c r="A31" s="9">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C31" s="4">
         <f t="shared" si="1"/>
         <v>56</v>
       </c>
-      <c r="D31" s="1">
-        <f t="shared" si="2"/>
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="E31" s="1">
+      <c r="D31" s="4">
+        <f t="shared" si="2"/>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E31" s="4">
         <f>Таблица2[[#This Row],[Столбец3]]*Таблица2[[#This Row],[Столбец4]]</f>
         <v>246.40000000000003</v>
       </c>
@@ -1928,39 +1959,39 @@
         <f t="shared" si="3"/>
         <v>44833</v>
       </c>
-      <c r="H31" s="1">
+      <c r="H31" s="4">
         <f t="shared" si="4"/>
         <v>20</v>
       </c>
-      <c r="I31" s="1">
-        <v>10</v>
-      </c>
-      <c r="J31" s="1">
+      <c r="I31" s="4">
+        <v>10</v>
+      </c>
+      <c r="J31" s="4">
         <f>Таблица2[[#This Row],[Столбец9]]*Таблица2[[#This Row],[Столбец8]]</f>
         <v>200</v>
       </c>
-      <c r="K31" s="1">
+      <c r="K31" s="4">
         <f>Таблица2[[#This Row],[Столбец10]]+Таблица2[[#This Row],[Столбец5]]</f>
         <v>446.40000000000003</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
+      <c r="A32" s="9">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C32" s="1">
+      <c r="C32" s="4">
         <f t="shared" si="1"/>
         <v>55.5</v>
       </c>
-      <c r="D32" s="1">
-        <f t="shared" si="2"/>
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="E32" s="1">
+      <c r="D32" s="4">
+        <f t="shared" si="2"/>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E32" s="4">
         <f>Таблица2[[#This Row],[Столбец3]]*Таблица2[[#This Row],[Столбец4]]</f>
         <v>244.20000000000002</v>
       </c>
@@ -1971,39 +2002,39 @@
         <f>G31+1</f>
         <v>44834</v>
       </c>
-      <c r="H32" s="1">
+      <c r="H32" s="4">
         <f t="shared" si="4"/>
         <v>21</v>
       </c>
-      <c r="I32" s="1">
-        <v>10</v>
-      </c>
-      <c r="J32" s="1">
+      <c r="I32" s="4">
+        <v>10</v>
+      </c>
+      <c r="J32" s="4">
         <f>Таблица2[[#This Row],[Столбец9]]*Таблица2[[#This Row],[Столбец8]]</f>
         <v>210</v>
       </c>
-      <c r="K32" s="1">
+      <c r="K32" s="4">
         <f>Таблица2[[#This Row],[Столбец10]]+Таблица2[[#This Row],[Столбец5]]</f>
         <v>454.20000000000005</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="2">
+      <c r="A33" s="9">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C33" s="4">
         <f t="shared" si="1"/>
         <v>55</v>
       </c>
-      <c r="D33" s="1">
-        <f t="shared" si="2"/>
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="E33" s="1">
+      <c r="D33" s="4">
+        <f t="shared" si="2"/>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E33" s="4">
         <f>Таблица2[[#This Row],[Столбец3]]*Таблица2[[#This Row],[Столбец4]]</f>
         <v>242.00000000000003</v>
       </c>
@@ -2013,39 +2044,39 @@
       <c r="G33" s="7">
         <v>44835</v>
       </c>
-      <c r="H33" s="1">
+      <c r="H33" s="4">
         <f t="shared" si="4"/>
         <v>22</v>
       </c>
-      <c r="I33" s="1">
-        <v>10</v>
-      </c>
-      <c r="J33" s="1">
+      <c r="I33" s="4">
+        <v>10</v>
+      </c>
+      <c r="J33" s="4">
         <f>Таблица2[[#This Row],[Столбец9]]*Таблица2[[#This Row],[Столбец8]]</f>
         <v>220</v>
       </c>
-      <c r="K33" s="1">
+      <c r="K33" s="4">
         <f>Таблица2[[#This Row],[Столбец10]]+Таблица2[[#This Row],[Столбец5]]</f>
         <v>462</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="2">
+      <c r="A34" s="9">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C34" s="1">
+      <c r="C34" s="4">
         <f t="shared" si="1"/>
         <v>54.5</v>
       </c>
-      <c r="D34" s="1">
-        <f t="shared" si="2"/>
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="E34" s="1">
+      <c r="D34" s="4">
+        <f t="shared" si="2"/>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E34" s="4">
         <f>Таблица2[[#This Row],[Столбец3]]*Таблица2[[#This Row],[Столбец4]]</f>
         <v>239.8</v>
       </c>
@@ -2056,39 +2087,39 @@
         <f>G33+1</f>
         <v>44836</v>
       </c>
-      <c r="H34" s="1">
+      <c r="H34" s="4">
         <f t="shared" si="4"/>
         <v>23</v>
       </c>
-      <c r="I34" s="1">
-        <v>10</v>
-      </c>
-      <c r="J34" s="1">
+      <c r="I34" s="4">
+        <v>10</v>
+      </c>
+      <c r="J34" s="4">
         <f>Таблица2[[#This Row],[Столбец9]]*Таблица2[[#This Row],[Столбец8]]</f>
         <v>230</v>
       </c>
-      <c r="K34" s="1">
+      <c r="K34" s="4">
         <f>Таблица2[[#This Row],[Столбец10]]+Таблица2[[#This Row],[Столбец5]]</f>
         <v>469.8</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="2">
+      <c r="A35" s="9">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C35" s="4">
         <f t="shared" si="1"/>
         <v>54</v>
       </c>
-      <c r="D35" s="1">
-        <f t="shared" si="2"/>
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="E35" s="1">
+      <c r="D35" s="4">
+        <f t="shared" si="2"/>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E35" s="4">
         <f>Таблица2[[#This Row],[Столбец3]]*Таблица2[[#This Row],[Столбец4]]</f>
         <v>237.60000000000002</v>
       </c>
@@ -2099,39 +2130,39 @@
         <f t="shared" ref="G35:G38" si="5">G34+1</f>
         <v>44837</v>
       </c>
-      <c r="H35" s="1">
+      <c r="H35" s="4">
         <f t="shared" si="4"/>
         <v>24</v>
       </c>
-      <c r="I35" s="1">
-        <v>10</v>
-      </c>
-      <c r="J35" s="1">
+      <c r="I35" s="4">
+        <v>10</v>
+      </c>
+      <c r="J35" s="4">
         <f>Таблица2[[#This Row],[Столбец9]]*Таблица2[[#This Row],[Столбец8]]</f>
         <v>240</v>
       </c>
-      <c r="K35" s="1">
+      <c r="K35" s="4">
         <f>Таблица2[[#This Row],[Столбец10]]+Таблица2[[#This Row],[Столбец5]]</f>
         <v>477.6</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="2">
+      <c r="A36" s="9">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C36" s="1">
+      <c r="C36" s="4">
         <f t="shared" si="1"/>
         <v>53.5</v>
       </c>
-      <c r="D36" s="1">
-        <f t="shared" si="2"/>
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="E36" s="1">
+      <c r="D36" s="4">
+        <f t="shared" si="2"/>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E36" s="4">
         <f>Таблица2[[#This Row],[Столбец3]]*Таблица2[[#This Row],[Столбец4]]</f>
         <v>235.4</v>
       </c>
@@ -2142,39 +2173,39 @@
         <f t="shared" si="5"/>
         <v>44838</v>
       </c>
-      <c r="H36" s="1">
+      <c r="H36" s="4">
         <f t="shared" si="4"/>
         <v>25</v>
       </c>
-      <c r="I36" s="1">
-        <v>10</v>
-      </c>
-      <c r="J36" s="1">
+      <c r="I36" s="4">
+        <v>10</v>
+      </c>
+      <c r="J36" s="4">
         <f>Таблица2[[#This Row],[Столбец9]]*Таблица2[[#This Row],[Столбец8]]</f>
         <v>250</v>
       </c>
-      <c r="K36" s="1">
+      <c r="K36" s="4">
         <f>Таблица2[[#This Row],[Столбец10]]+Таблица2[[#This Row],[Столбец5]]</f>
         <v>485.4</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="2">
+      <c r="A37" s="9">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C37" s="1">
+      <c r="C37" s="4">
         <f t="shared" si="1"/>
         <v>53</v>
       </c>
-      <c r="D37" s="1">
-        <f t="shared" si="2"/>
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="E37" s="1">
+      <c r="D37" s="4">
+        <f t="shared" si="2"/>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E37" s="4">
         <f>Таблица2[[#This Row],[Столбец3]]*Таблица2[[#This Row],[Столбец4]]</f>
         <v>233.20000000000002</v>
       </c>
@@ -2185,39 +2216,39 @@
         <f t="shared" si="5"/>
         <v>44839</v>
       </c>
-      <c r="H37" s="1">
+      <c r="H37" s="4">
         <f t="shared" si="4"/>
         <v>26</v>
       </c>
-      <c r="I37" s="1">
-        <v>10</v>
-      </c>
-      <c r="J37" s="1">
+      <c r="I37" s="4">
+        <v>10</v>
+      </c>
+      <c r="J37" s="4">
         <f>Таблица2[[#This Row],[Столбец9]]*Таблица2[[#This Row],[Столбец8]]</f>
         <v>260</v>
       </c>
-      <c r="K37" s="1">
+      <c r="K37" s="4">
         <f>Таблица2[[#This Row],[Столбец10]]+Таблица2[[#This Row],[Столбец5]]</f>
         <v>493.20000000000005</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="2">
+      <c r="A38" s="10">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C38" s="1">
+      <c r="C38" s="4">
         <f t="shared" si="1"/>
         <v>52.5</v>
       </c>
-      <c r="D38" s="1">
-        <f t="shared" si="2"/>
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="E38" s="1">
+      <c r="D38" s="4">
+        <f t="shared" si="2"/>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E38" s="4">
         <f>Таблица2[[#This Row],[Столбец3]]*Таблица2[[#This Row],[Столбец4]]</f>
         <v>231.00000000000003</v>
       </c>
@@ -2228,54 +2259,54 @@
         <f t="shared" si="5"/>
         <v>44840</v>
       </c>
-      <c r="H38" s="1">
+      <c r="H38" s="4">
         <f t="shared" si="4"/>
         <v>27</v>
       </c>
-      <c r="I38" s="1">
-        <v>10</v>
-      </c>
-      <c r="J38" s="1">
+      <c r="I38" s="4">
+        <v>10</v>
+      </c>
+      <c r="J38" s="4">
         <f>Таблица2[[#This Row],[Столбец9]]*Таблица2[[#This Row],[Столбец8]]</f>
         <v>270</v>
       </c>
-      <c r="K38" s="1">
+      <c r="K38" s="4">
         <f>Таблица2[[#This Row],[Столбец10]]+Таблица2[[#This Row],[Столбец5]]</f>
         <v>501</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B40" s="1" t="s">
+      <c r="B40" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C40" s="1">
-        <f>SUM(K3:K38)</f>
+      <c r="C40" s="11">
+        <f>ROUNDDOWN(SUM(K3:K38),0)</f>
         <v>13482</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B41" s="1" t="s">
+      <c r="B41" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C41" s="1">
+      <c r="C41" s="11">
         <f>AVERAGE(C3:C38)</f>
         <v>61.25</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B42" s="1" t="s">
+      <c r="B42" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C42" s="1">
+      <c r="C42" s="4">
         <f>MAX(H3:H38)</f>
         <v>27</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B43" s="1" t="s">
+      <c r="B43" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C43" s="1">
+      <c r="C43" s="12">
         <f>MAX(K3:K38)</f>
         <v>501</v>
       </c>

</xml_diff>